<commit_message>
Atualizado por script em 24-11-2023 02:45
</commit_message>
<xml_diff>
--- a/2023/chile_primera-division_2023.xlsx
+++ b/2023/chile_primera-division_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V215"/>
+  <dimension ref="A1:V216"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20237,6 +20237,98 @@
         </is>
       </c>
     </row>
+    <row r="216">
+      <c r="A216" s="1" t="n">
+        <v>215</v>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>chile</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>primera-division</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E216" s="2" t="n">
+        <v>45253.91666666666</v>
+      </c>
+      <c r="F216" t="inlineStr">
+        <is>
+          <t>Palestino</t>
+        </is>
+      </c>
+      <c r="G216" t="n">
+        <v>0</v>
+      </c>
+      <c r="H216" t="inlineStr">
+        <is>
+          <t>Everton</t>
+        </is>
+      </c>
+      <c r="I216" t="n">
+        <v>2</v>
+      </c>
+      <c r="J216" t="n">
+        <v>2.03</v>
+      </c>
+      <c r="K216" t="inlineStr">
+        <is>
+          <t>16/11/2023 22:12</t>
+        </is>
+      </c>
+      <c r="L216" t="n">
+        <v>1.87</v>
+      </c>
+      <c r="M216" t="inlineStr">
+        <is>
+          <t>23/11/2023 21:59</t>
+        </is>
+      </c>
+      <c r="N216" t="n">
+        <v>3.53</v>
+      </c>
+      <c r="O216" t="inlineStr">
+        <is>
+          <t>16/11/2023 22:12</t>
+        </is>
+      </c>
+      <c r="P216" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="Q216" t="inlineStr">
+        <is>
+          <t>23/11/2023 21:59</t>
+        </is>
+      </c>
+      <c r="R216" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="S216" t="inlineStr">
+        <is>
+          <t>16/11/2023 22:12</t>
+        </is>
+      </c>
+      <c r="T216" t="n">
+        <v>4.22</v>
+      </c>
+      <c r="U216" t="inlineStr">
+        <is>
+          <t>23/11/2023 21:59</t>
+        </is>
+      </c>
+      <c r="V216" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/chile/primera-division/palestino-everton/jT9tS3EN/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizado por script em 02-12-2023 02:45
</commit_message>
<xml_diff>
--- a/2023/chile_primera-division_2023.xlsx
+++ b/2023/chile_primera-division_2023.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V223"/>
+  <dimension ref="A1:V224"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9221,71 +9221,71 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>U. Espanola</t>
+          <t>Nublense</t>
         </is>
       </c>
       <c r="G96" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>Union La Calera</t>
+          <t>Copiapo</t>
         </is>
       </c>
       <c r="I96" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J96" t="n">
-        <v>2.46</v>
+        <v>1.83</v>
       </c>
       <c r="K96" t="inlineStr">
         <is>
-          <t>01/05/2023 00:12</t>
+          <t>03/05/2023 00:12</t>
         </is>
       </c>
       <c r="L96" t="n">
-        <v>2.59</v>
+        <v>1.92</v>
       </c>
       <c r="M96" t="inlineStr">
         <is>
+          <t>09/05/2023 23:59</t>
+        </is>
+      </c>
+      <c r="N96" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>03/05/2023 00:12</t>
+        </is>
+      </c>
+      <c r="P96" t="n">
+        <v>3.59</v>
+      </c>
+      <c r="Q96" t="inlineStr">
+        <is>
           <t>09/05/2023 23:58</t>
         </is>
       </c>
-      <c r="N96" t="n">
-        <v>3.26</v>
-      </c>
-      <c r="O96" t="inlineStr">
-        <is>
-          <t>01/05/2023 00:12</t>
-        </is>
-      </c>
-      <c r="P96" t="n">
-        <v>3.32</v>
-      </c>
-      <c r="Q96" t="inlineStr">
-        <is>
-          <t>09/05/2023 23:58</t>
-        </is>
-      </c>
       <c r="R96" t="n">
-        <v>2.88</v>
+        <v>3.97</v>
       </c>
       <c r="S96" t="inlineStr">
         <is>
-          <t>01/05/2023 00:12</t>
+          <t>03/05/2023 00:12</t>
         </is>
       </c>
       <c r="T96" t="n">
-        <v>2.9</v>
+        <v>4.26</v>
       </c>
       <c r="U96" t="inlineStr">
         <is>
-          <t>09/05/2023 23:58</t>
+          <t>09/05/2023 23:59</t>
         </is>
       </c>
       <c r="V96" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/chile/primera-division/u-espanola-union-la-calera/ANNl21xB/</t>
+          <t>https://www.betexplorer.com/football/chile/primera-division/nublense-copiapo/WWOp3sN4/</t>
         </is>
       </c>
     </row>
@@ -9313,46 +9313,46 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Nublense</t>
+          <t>U. Espanola</t>
         </is>
       </c>
       <c r="G97" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>Copiapo</t>
+          <t>Union La Calera</t>
         </is>
       </c>
       <c r="I97" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J97" t="n">
-        <v>1.83</v>
+        <v>2.46</v>
       </c>
       <c r="K97" t="inlineStr">
         <is>
-          <t>03/05/2023 00:12</t>
+          <t>01/05/2023 00:12</t>
         </is>
       </c>
       <c r="L97" t="n">
-        <v>1.92</v>
+        <v>2.59</v>
       </c>
       <c r="M97" t="inlineStr">
         <is>
-          <t>09/05/2023 23:59</t>
+          <t>09/05/2023 23:58</t>
         </is>
       </c>
       <c r="N97" t="n">
-        <v>3.76</v>
+        <v>3.26</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
-          <t>03/05/2023 00:12</t>
+          <t>01/05/2023 00:12</t>
         </is>
       </c>
       <c r="P97" t="n">
-        <v>3.59</v>
+        <v>3.32</v>
       </c>
       <c r="Q97" t="inlineStr">
         <is>
@@ -9360,24 +9360,24 @@
         </is>
       </c>
       <c r="R97" t="n">
-        <v>3.97</v>
+        <v>2.88</v>
       </c>
       <c r="S97" t="inlineStr">
         <is>
-          <t>03/05/2023 00:12</t>
+          <t>01/05/2023 00:12</t>
         </is>
       </c>
       <c r="T97" t="n">
-        <v>4.26</v>
+        <v>2.9</v>
       </c>
       <c r="U97" t="inlineStr">
         <is>
-          <t>09/05/2023 23:59</t>
+          <t>09/05/2023 23:58</t>
         </is>
       </c>
       <c r="V97" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/chile/primera-division/nublense-copiapo/WWOp3sN4/</t>
+          <t>https://www.betexplorer.com/football/chile/primera-division/u-espanola-union-la-calera/ANNl21xB/</t>
         </is>
       </c>
     </row>
@@ -20813,71 +20813,71 @@
       </c>
       <c r="F222" t="inlineStr">
         <is>
-          <t>Curico Unido</t>
+          <t>Copiapo</t>
         </is>
       </c>
       <c r="G222" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H222" t="inlineStr">
         <is>
-          <t>Magallanes</t>
+          <t>Nublense</t>
         </is>
       </c>
       <c r="I222" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J222" t="n">
-        <v>2.01</v>
+        <v>2.49</v>
       </c>
       <c r="K222" t="inlineStr">
         <is>
-          <t>19/11/2023 03:43</t>
+          <t>19/11/2023 03:42</t>
         </is>
       </c>
       <c r="L222" t="n">
-        <v>2.66</v>
+        <v>2.8</v>
       </c>
       <c r="M222" t="inlineStr">
         <is>
-          <t>27/11/2023 00:30</t>
+          <t>27/11/2023 00:26</t>
         </is>
       </c>
       <c r="N222" t="n">
-        <v>3.56</v>
+        <v>3.47</v>
       </c>
       <c r="O222" t="inlineStr">
         <is>
-          <t>19/11/2023 03:43</t>
+          <t>19/11/2023 03:42</t>
         </is>
       </c>
       <c r="P222" t="n">
-        <v>3.63</v>
+        <v>3.2</v>
       </c>
       <c r="Q222" t="inlineStr">
         <is>
-          <t>27/11/2023 00:00</t>
+          <t>27/11/2023 00:26</t>
         </is>
       </c>
       <c r="R222" t="n">
-        <v>3.51</v>
+        <v>2.92</v>
       </c>
       <c r="S222" t="inlineStr">
         <is>
-          <t>19/11/2023 03:43</t>
+          <t>19/11/2023 03:42</t>
         </is>
       </c>
       <c r="T222" t="n">
-        <v>2.62</v>
+        <v>2.76</v>
       </c>
       <c r="U222" t="inlineStr">
         <is>
-          <t>27/11/2023 00:30</t>
+          <t>27/11/2023 00:26</t>
         </is>
       </c>
       <c r="V222" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/chile/primera-division/curico-unido-magallanes/8pjDMsxo/</t>
+          <t>https://www.betexplorer.com/football/chile/primera-division/copiapo-nublense/MmveoREo/</t>
         </is>
       </c>
     </row>
@@ -20905,71 +20905,163 @@
       </c>
       <c r="F223" t="inlineStr">
         <is>
-          <t>Copiapo</t>
+          <t>Curico Unido</t>
         </is>
       </c>
       <c r="G223" t="n">
+        <v>3</v>
+      </c>
+      <c r="H223" t="inlineStr">
+        <is>
+          <t>Magallanes</t>
+        </is>
+      </c>
+      <c r="I223" t="n">
+        <v>4</v>
+      </c>
+      <c r="J223" t="n">
+        <v>2.01</v>
+      </c>
+      <c r="K223" t="inlineStr">
+        <is>
+          <t>19/11/2023 03:43</t>
+        </is>
+      </c>
+      <c r="L223" t="n">
+        <v>2.66</v>
+      </c>
+      <c r="M223" t="inlineStr">
+        <is>
+          <t>27/11/2023 00:30</t>
+        </is>
+      </c>
+      <c r="N223" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="O223" t="inlineStr">
+        <is>
+          <t>19/11/2023 03:43</t>
+        </is>
+      </c>
+      <c r="P223" t="n">
+        <v>3.63</v>
+      </c>
+      <c r="Q223" t="inlineStr">
+        <is>
+          <t>27/11/2023 00:00</t>
+        </is>
+      </c>
+      <c r="R223" t="n">
+        <v>3.51</v>
+      </c>
+      <c r="S223" t="inlineStr">
+        <is>
+          <t>19/11/2023 03:43</t>
+        </is>
+      </c>
+      <c r="T223" t="n">
+        <v>2.62</v>
+      </c>
+      <c r="U223" t="inlineStr">
+        <is>
+          <t>27/11/2023 00:30</t>
+        </is>
+      </c>
+      <c r="V223" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/chile/primera-division/curico-unido-magallanes/8pjDMsxo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="1" t="n">
+        <v>223</v>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>chile</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>primera-division</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="E224" s="2" t="n">
+        <v>45262</v>
+      </c>
+      <c r="F224" t="inlineStr">
+        <is>
+          <t>Coquimbo</t>
+        </is>
+      </c>
+      <c r="G224" t="n">
         <v>1</v>
       </c>
-      <c r="H223" t="inlineStr">
-        <is>
-          <t>Nublense</t>
-        </is>
-      </c>
-      <c r="I223" t="n">
-        <v>1</v>
-      </c>
-      <c r="J223" t="n">
-        <v>2.49</v>
-      </c>
-      <c r="K223" t="inlineStr">
-        <is>
-          <t>19/11/2023 03:42</t>
-        </is>
-      </c>
-      <c r="L223" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="M223" t="inlineStr">
-        <is>
-          <t>27/11/2023 00:26</t>
-        </is>
-      </c>
-      <c r="N223" t="n">
-        <v>3.47</v>
-      </c>
-      <c r="O223" t="inlineStr">
-        <is>
-          <t>19/11/2023 03:42</t>
-        </is>
-      </c>
-      <c r="P223" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="Q223" t="inlineStr">
-        <is>
-          <t>27/11/2023 00:26</t>
-        </is>
-      </c>
-      <c r="R223" t="n">
-        <v>2.92</v>
-      </c>
-      <c r="S223" t="inlineStr">
-        <is>
-          <t>19/11/2023 03:42</t>
-        </is>
-      </c>
-      <c r="T223" t="n">
-        <v>2.76</v>
-      </c>
-      <c r="U223" t="inlineStr">
-        <is>
-          <t>27/11/2023 00:26</t>
-        </is>
-      </c>
-      <c r="V223" t="inlineStr">
-        <is>
-          <t>https://www.betexplorer.com/football/chile/primera-division/copiapo-nublense/MmveoREo/</t>
+      <c r="H224" t="inlineStr">
+        <is>
+          <t>Union La Calera</t>
+        </is>
+      </c>
+      <c r="I224" t="n">
+        <v>2</v>
+      </c>
+      <c r="J224" t="n">
+        <v>2.23</v>
+      </c>
+      <c r="K224" t="inlineStr">
+        <is>
+          <t>25/11/2023 00:42</t>
+        </is>
+      </c>
+      <c r="L224" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="M224" t="inlineStr">
+        <is>
+          <t>01/12/2023 23:51</t>
+        </is>
+      </c>
+      <c r="N224" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="O224" t="inlineStr">
+        <is>
+          <t>25/11/2023 00:42</t>
+        </is>
+      </c>
+      <c r="P224" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="Q224" t="inlineStr">
+        <is>
+          <t>01/12/2023 23:51</t>
+        </is>
+      </c>
+      <c r="R224" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="S224" t="inlineStr">
+        <is>
+          <t>25/11/2023 00:42</t>
+        </is>
+      </c>
+      <c r="T224" t="n">
+        <v>3.34</v>
+      </c>
+      <c r="U224" t="inlineStr">
+        <is>
+          <t>01/12/2023 23:54</t>
+        </is>
+      </c>
+      <c r="V224" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/chile/primera-division/coquimbo-union-la-calera/d6W7rPb4/</t>
         </is>
       </c>
     </row>

</xml_diff>